<commit_message>
Updated some, but it is shit
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>V1是动态生成ViewModel（按下按钮后生成），也是再ResourcesDictionary里面动态绑定。V2没有动态生成页面，所以也不需要动态绑定。整体结构是：MainWindow包含多个子控件。MainWindow的DataContext设为MainWindowViewModel。MainWindow.SubControl.DataContext = MainWindowViewModel.SubControlViewModel</t>
+  </si>
+  <si>
+    <t>制作Model部分的类结构图，并与Kyle Review</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -431,7 +437,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C12:C14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -477,6 +483,12 @@
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="75">
       <c r="A4" s="1">

</xml_diff>

<commit_message>
Fixed Execute and Commit issues
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,9 +62,6 @@
     <t>制作Model部分的类结构图，并与Kyle Review</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>Close</t>
   </si>
   <si>
@@ -91,13 +88,26 @@
   </si>
   <si>
     <t>cannot delete relatation??</t>
+  </si>
+  <si>
+    <t>Add的时候没有加到runtime的model里。</t>
+  </si>
+  <si>
+    <t>initialize的时候将models传进来。Add的时候不仅将newm放到DB里去，也要放到models里面去。</t>
+  </si>
+  <si>
+    <t>Modify了某个BatteryType的Name，但是在其他View看不到这个修改，但是其实数据库里是已经修改了的.
+其他类似情况包括修改TesterName之后，在Channel的Tester项中看不到这个修改，等</t>
+  </si>
+  <si>
+    <t>Execute某个TR，Commit这个TR，会因为找不到Assets而crash.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,13 +121,6 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,14 +140,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -152,15 +151,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -478,17 +473,17 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -533,7 +528,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -544,7 +539,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="75">
@@ -566,32 +561,52 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="60">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>22</v>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue6 for subprogramtemplate
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,6 +62,9 @@
     <t>制作Model部分的类结构图，并与Kyle Review</t>
   </si>
   <si>
+    <t>Open</t>
+  </si>
+  <si>
     <t>Close</t>
   </si>
   <si>
@@ -116,6 +119,15 @@
   </si>
   <si>
     <t>调整model赋值顺序，在savechanges之后赋值</t>
+  </si>
+  <si>
+    <t>Re-open</t>
+  </si>
+  <si>
+    <t>Commit没有改变Assets在m和vm中的状态（DB已改）</t>
+  </si>
+  <si>
+    <t>如果Execute,Complete连续执行，Assets的Status会正常变化。如果Execute之后关闭再重启程序，再进行Commit, Assets的Status不会变化</t>
   </si>
 </sst>
 </file>
@@ -468,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -489,16 +501,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -543,7 +555,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -554,7 +566,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="75">
@@ -576,13 +588,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>2</v>
@@ -593,7 +605,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30">
@@ -601,19 +616,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -621,7 +636,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -629,13 +644,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>2</v>
@@ -646,10 +661,24 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create db at runtime
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>调整model赋值顺序，在savechanges之后赋值</t>
-  </si>
-  <si>
-    <t>Re-open</t>
   </si>
   <si>
     <t>Commit没有改变Assets在m和vm中的状态（DB已改）</t>
@@ -483,7 +480,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -625,7 +622,7 @@
         <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>22</v>
@@ -675,10 +672,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Same context, fixed issue 12
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t>Navigation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在从DB取出m的时候，用了多个context。例如某个battery,在Batteries = dbContext.Batteries…的时候加载了一次，在programs.subprograms.testrecords.assignedbattery的时候又加载了一次。而这两次加载位于不同的context，所以即使他们的id相同，但他们其实是不同的instance。于是，BatteryVM绑定了model1的事件，而ProgramVM使得model2发出事件,并不会通知BatteryVM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在同一个context中加载model，这样battery和programs.subprograms.testrecords.assignedbattery就是同一个instance.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -537,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -733,7 +745,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="108" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -743,8 +755,14 @@
       <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="F14" s="1" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -758,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed issue 11 with solution 1, fixed issue 13
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -112,9 +112,6 @@
     <t>model没有利用到SaveChanges的side effect</t>
   </si>
   <si>
-    <t>重启后Invalid不起效</t>
-  </si>
-  <si>
     <t>调整model赋值顺序，在savechanges之后赋值</t>
   </si>
   <si>
@@ -149,10 +146,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>如果Execute,Complete,Invalid连续执行，Invalid可正常工作。如果Commit之后关闭再重启程序，再进行Invalid，会失效</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Records</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -174,6 +167,47 @@
   </si>
   <si>
     <t>Fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重启后Invalid不起效（DB也未改）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果Create,Execute,Complete,Invalid连续执行，Invalid可正常工作。如果过程中关闭再重启程序，再继续进行到Invalid，会发现Invalid失效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二次Invalid不起效（DB也未改）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果Create,Execute,Complete,Invalid连续执行，Invalid可正常工作（添加了新的testrecord）。这时如果再次将新的testrecord Invalidate，会发现Invalidate失效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看代码发现，subprogram订阅tr的status changed event，发生在以下情况：
+1. proeditVM.add-&gt;sub.constructe
+2. prosVM.edit||prosVM.saveas-&gt;sub.clone
+如果没有在UI上进行以上操作，就不会有订阅。而从DB中捞出model的时候，本身是不会带有订阅信息的。所以只有新动作产生的model会有符合预期的行为。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.从DB捞出model的时候，重新建立订阅关系
+2.不要使用事件来实现invalidate功能。直接在sub层面实现Invalidate.
+使用了方案1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在sub的响应函数中，添加新的tr，但是忘了订阅新tr的事件。所以不能响应新tr的事件。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加新tr的时候，订阅新tr的事件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -197,7 +231,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +241,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -223,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -244,6 +296,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -547,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -584,69 +651,80 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="1">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="1">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A4" s="1">
+    <row r="4" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="1">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A6" s="1">
+    <row r="6" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="11" t="s">
         <v>2</v>
       </c>
     </row>
@@ -658,20 +736,21 @@
       <c r="E7" s="7"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:7" ht="54" x14ac:dyDescent="0.15">
-      <c r="A8" s="1">
+    <row r="8" spans="1:7" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+      <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="9" t="s">
         <v>2</v>
       </c>
     </row>
@@ -687,82 +766,114 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="A10" s="1">
+      <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="1">
+    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A11" s="9">
         <v>9</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10" t="s">
         <v>26</v>
       </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="1">
+      <c r="A12" s="9">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="108" x14ac:dyDescent="0.15">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="C14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A15" s="9">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="108" x14ac:dyDescent="0.15">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>45</v>
+      <c r="B15" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -777,7 +888,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -811,13 +922,8 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4" t="s">
-        <v>34</v>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -825,7 +931,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -833,7 +939,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -841,7 +947,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -857,7 +963,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -865,15 +971,20 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>42</v>
+      <c r="B9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add app.manifest to grant administrator previleges
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -208,6 +208,41 @@
   </si>
   <si>
     <t>添加新tr的时候，订阅新tr的事件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deployment Issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在VM上无法运行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缺乏权限无法创建DB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用app.manifest提升权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无需询问权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIXED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slice must be between 0.0 and 1.0.</t>
+  </si>
+  <si>
+    <t>若使用新DB则无法启动程序</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -614,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -876,6 +911,45 @@
         <v>50</v>
       </c>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -888,7 +962,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -924,6 +998,9 @@
       </c>
       <c r="B2" s="4" t="s">
         <v>37</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Fixed Raw Data List Import and display
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Issues" sheetId="1" r:id="rId1"/>
-    <sheet name="Features" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Features" sheetId="2" r:id="rId1"/>
+    <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -297,22 +296,41 @@
     <t>第一次运行时DashBoard不更新</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Upload to server</t>
+  </si>
+  <si>
+    <t>DB部署问题</t>
+  </si>
+  <si>
+    <t>目前DB是放在C盘的，这个有很大的隐患。例如有些用户没有C盘权限之类的。</t>
+  </si>
+  <si>
+    <t>启动时，检查配置文件。如果配置文件不存在，表示从未进行过配置。弹出窗口，让用户配置DB。用户选择使用已经存在的DB，或选择新建DB。程序按用户设定关联或创建DB，保存配置文件。</t>
+  </si>
+  <si>
+    <t>导入RawData</t>
+  </si>
+  <si>
+    <t>对于某些Test来说，RawData很大，无法放到一个文件中。例如aging test。因此，TestRecord要包含List&lt;RawData&gt;而不是单个RawData.
+Commit窗口的Browse按钮应该可以选择多个files。然后将这单个或多个file转换成rawdata，关联到TestRecord去。</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -402,7 +420,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -415,7 +433,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -489,7 +507,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -524,7 +541,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -700,24 +716,153 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9" style="4"/>
+    <col min="2" max="2" width="27.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4">
+        <v>4</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="46.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.75" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="60.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="60.85546875" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -737,7 +882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -753,7 +898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -769,7 +914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="105">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -785,7 +930,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -799,7 +944,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="105">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -815,7 +960,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -823,7 +968,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:7" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" s="8" customFormat="1" ht="90">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -841,7 +986,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="54" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="75">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -852,7 +997,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="30">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -873,7 +1018,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="30">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -885,7 +1030,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -903,7 +1048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="120">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -923,7 +1068,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="108" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="135">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -943,7 +1088,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="45">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -963,7 +1108,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -983,15 +1128,18 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="F17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30">
       <c r="A18" s="9">
         <v>16</v>
       </c>
@@ -1011,21 +1159,25 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A19" s="1">
+    <row r="19" spans="1:6" ht="135">
+      <c r="A19" s="9">
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="10" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="F19" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="120">
       <c r="A20" s="9">
         <v>18</v>
       </c>
@@ -1045,7 +1197,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6">
       <c r="A21" s="9">
         <v>19</v>
       </c>
@@ -1059,12 +1211,45 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>73</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="60">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="90">
+      <c r="A24" s="9">
+        <v>22</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1072,130 +1257,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="9" style="4"/>
-    <col min="2" max="2" width="27.625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="32.75" style="4" customWidth="1"/>
-    <col min="4" max="4" width="27" style="4" customWidth="1"/>
-    <col min="5" max="5" width="19.5" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
DB config process, sort list view
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="83">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -297,16 +297,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Upload to server</t>
-  </si>
-  <si>
     <t>DB部署问题</t>
   </si>
   <si>
     <t>目前DB是放在C盘的，这个有很大的隐患。例如有些用户没有C盘权限之类的。</t>
-  </si>
-  <si>
-    <t>启动时，检查配置文件。如果配置文件不存在，表示从未进行过配置。弹出窗口，让用户配置DB。用户选择使用已经存在的DB，或选择新建DB。程序按用户设定关联或创建DB，保存配置文件。</t>
   </si>
   <si>
     <t>导入RawData</t>
@@ -314,13 +308,29 @@
   <si>
     <t>对于某些Test来说，RawData很大，无法放到一个文件中。例如aging test。因此，TestRecord要包含List&lt;RawData&gt;而不是单个RawData.
 Commit窗口的Browse按钮应该可以选择多个files。然后将这单个或多个file转换成rawdata，关联到TestRecord去。</t>
+  </si>
+  <si>
+    <t>FIXED</t>
+  </si>
+  <si>
+    <t>Abandon</t>
+  </si>
+  <si>
+    <t>新创建的Assets在Dashboad这边不会变using</t>
+  </si>
+  <si>
+    <t>启动时，检查配置文件。如果配置文件不存在，表示从未进行过配置。弹出窗口，让用户配置DB。用户选择使用已经存在的DB，或选择新建DB。程序按用户设定关联或创建DB，保存配置文件。
+如果配置文件存在，则从配置文件中导入DB路径，然后按此路径使用DB</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/dotnet/framework/wpf/data/how-to-sort-and-group-data-using-a-view-in-xaml</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +344,13 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -377,10 +394,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -418,8 +439,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -430,6 +461,58 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>72265</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="647700" y="2514600"/>
+          <a:ext cx="6758815" cy="5095875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -717,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -731,7 +814,7 @@
     <col min="4" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -742,114 +825,124 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="4">
+    <row r="2" spans="1:4">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="4">
+    <row r="3" spans="1:4">
+      <c r="A3" s="14">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>34</v>
+      <c r="B3" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="4">
-        <v>5</v>
+    <row r="4" spans="1:4">
+      <c r="A4" s="14">
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
+      <c r="A5" s="14">
+        <v>4</v>
+      </c>
       <c r="B5" s="4" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="4">
-        <v>8</v>
-      </c>
-      <c r="B7" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="14">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="14">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="C7" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="4">
-        <v>6</v>
+        <v>78</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="14">
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="4">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="4">
-        <v>3</v>
-      </c>
-      <c r="B10" s="4" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" s="14">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="4">
-        <v>4</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="C9" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="14">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>33</v>
+      <c r="C10" s="13" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1222,18 +1315,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="60">
-      <c r="A23" s="1">
+    <row r="23" spans="1:6" ht="90">
+      <c r="A23" s="9">
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>77</v>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="90">
@@ -1241,15 +1338,20 @@
         <v>22</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="B25" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Assets Record display
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="86">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -324,6 +324,15 @@
   </si>
   <si>
     <t>https://docs.microsoft.com/en-us/dotnet/framework/wpf/data/how-to-sort-and-group-data-using-a-view-in-xaml</t>
+  </si>
+  <si>
+    <t>新的testrecord不会按降序添加</t>
+  </si>
+  <si>
+    <t>SubPrograms全屏，ProgramEditView拉宽，app拉宽</t>
+  </si>
+  <si>
+    <t>UI调整</t>
   </si>
 </sst>
 </file>
@@ -802,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -884,10 +893,10 @@
       <c r="A7" s="14">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="13" t="s">
         <v>78</v>
       </c>
       <c r="D7" s="15" t="s">
@@ -939,10 +948,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1350,8 +1359,35 @@
       </c>
     </row>
     <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
       <c r="B25" s="2" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Populate assets and programs
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,11 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="98">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -378,22 +377,25 @@
     <t>Fixed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Populate Historic Data</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -503,8 +505,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -569,7 +571,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -643,7 +645,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -678,7 +679,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -854,22 +854,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" style="4"/>
-    <col min="2" max="2" width="27.625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="4" customWidth="1"/>
     <col min="4" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -880,7 +880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -891,7 +891,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -902,7 +902,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -916,7 +916,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -927,7 +927,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -938,7 +938,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -952,7 +952,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7">
       <c r="A8" s="14">
         <v>7</v>
       </c>
@@ -963,7 +963,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7">
       <c r="A9" s="14">
         <v>8</v>
       </c>
@@ -974,7 +974,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -985,7 +985,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -996,7 +996,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1005,6 +1005,17 @@
       </c>
       <c r="C12" s="13" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1018,24 +1029,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="46.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.75" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="60.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="60.85546875" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1055,7 +1066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -1071,7 +1082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -1087,7 +1098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="105">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -1103,7 +1114,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -1117,7 +1128,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="105">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -1133,7 +1144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1141,7 +1152,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:7" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" s="8" customFormat="1" ht="90">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -1159,7 +1170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="54" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="75">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1170,7 +1181,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="30">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -1191,7 +1202,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="30">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -1203,7 +1214,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -1221,7 +1232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="120">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -1241,7 +1252,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="108" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="135">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -1261,7 +1272,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="45">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -1281,7 +1292,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -1301,7 +1312,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1312,7 +1323,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="30">
       <c r="A18" s="9">
         <v>16</v>
       </c>
@@ -1332,7 +1343,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="135">
       <c r="A19" s="9">
         <v>17</v>
       </c>
@@ -1350,7 +1361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="120">
       <c r="A20" s="9">
         <v>18</v>
       </c>
@@ -1370,7 +1381,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6">
       <c r="A21" s="9">
         <v>19</v>
       </c>
@@ -1384,7 +1395,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1395,7 +1406,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="54" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="90">
       <c r="A23" s="9">
         <v>21</v>
       </c>
@@ -1413,7 +1424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="54" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="90">
       <c r="A24" s="9">
         <v>22</v>
       </c>
@@ -1429,7 +1440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1437,7 +1448,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1445,7 +1456,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="30">
       <c r="A27" s="9">
         <v>25</v>
       </c>
@@ -1461,7 +1472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1469,7 +1480,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1477,7 +1488,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="30">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1485,7 +1496,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1493,7 +1504,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="54" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="60">
       <c r="A32" s="9">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Removed big blob data
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="101">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -382,6 +382,12 @@
   </si>
   <si>
     <t>xceed.wpf.toolkit.DateTimePicker</t>
+  </si>
+  <si>
+    <t>目前来说只能放到本地目录，因为OpenFileDialog看不到网络驱动器</t>
+  </si>
+  <si>
+    <t>历史操作还没实现</t>
   </si>
 </sst>
 </file>
@@ -860,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1020,6 +1026,9 @@
       <c r="C13" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="E13" s="4" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1033,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1315,7 +1324,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1326,7 +1335,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30">
+    <row r="18" spans="1:10" ht="30">
       <c r="A18" s="9">
         <v>16</v>
       </c>
@@ -1346,7 +1355,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="135">
+    <row r="19" spans="1:10" ht="135">
       <c r="A19" s="9">
         <v>17</v>
       </c>
@@ -1364,7 +1373,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="120">
+    <row r="20" spans="1:10" ht="120">
       <c r="A20" s="9">
         <v>18</v>
       </c>
@@ -1384,7 +1393,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:10">
       <c r="A21" s="9">
         <v>19</v>
       </c>
@@ -1398,7 +1407,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1409,7 +1418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="90">
+    <row r="23" spans="1:10" ht="90">
       <c r="A23" s="9">
         <v>21</v>
       </c>
@@ -1427,7 +1436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="90">
+    <row r="24" spans="1:10" ht="90">
       <c r="A24" s="9">
         <v>22</v>
       </c>
@@ -1443,7 +1452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1451,7 +1460,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1459,7 +1468,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30">
+    <row r="27" spans="1:10" ht="30">
       <c r="A27" s="9">
         <v>25</v>
       </c>
@@ -1475,7 +1484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1483,7 +1492,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:10">
       <c r="A29" s="9">
         <v>27</v>
       </c>
@@ -1499,15 +1508,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30">
-      <c r="A30" s="1">
+    <row r="30" spans="1:10" ht="30">
+      <c r="A30" s="9">
         <v>28</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="10" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1515,7 +1533,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="60">
+    <row r="32" spans="1:10" ht="60">
       <c r="A32" s="9">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Fixed openfiledialog cannot see network drive issue
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="107">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -222,10 +222,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>使用app.manifest提升权限</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Fixed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -353,10 +349,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Raw data并不直接放进数据库，而是关联起来就好</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Cycle更新</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -384,10 +376,34 @@
     <t>xceed.wpf.toolkit.DateTimePicker</t>
   </si>
   <si>
-    <t>目前来说只能放到本地目录，因为OpenFileDialog看不到网络驱动器</t>
-  </si>
-  <si>
     <t>历史操作还没实现</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>使用app.manifest提升权限(Fixed 21之后，不再需要此权限)</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>移除byte[] binarydata</t>
+  </si>
+  <si>
+    <t>Raw data并不直接放进数据库，而是关联文件路径就好</t>
+  </si>
+  <si>
+    <t>OpenFileDialog看不到网络驱动器</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/32790495/mapped-drives-not-visible-on-open-dialog</t>
+  </si>
+  <si>
+    <t>移除权限就好了</t>
+  </si>
+  <si>
+    <t>显示有点小问题</t>
   </si>
 </sst>
 </file>
@@ -417,7 +433,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,6 +464,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -465,7 +487,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -512,6 +534,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -866,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -897,7 +926,7 @@
         <v>37</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -905,7 +934,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>33</v>
@@ -922,7 +951,7 @@
         <v>33</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -933,7 +962,7 @@
         <v>38</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -955,10 +984,10 @@
         <v>39</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -980,7 +1009,7 @@
         <v>35</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -991,7 +1020,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -999,7 +1028,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>33</v>
@@ -1010,10 +1039,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1021,13 +1050,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1042,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1305,255 +1334,281 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="9">
+      <c r="A16" s="16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30">
+      <c r="A17" s="9">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="135">
+      <c r="A18" s="9">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="120">
+      <c r="A19" s="9">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="9">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="16">
         <v>14</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B22" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C22" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D22" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="30">
-      <c r="A18" s="9">
-        <v>16</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="135">
-      <c r="A19" s="9">
-        <v>17</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="120">
-      <c r="A20" s="9">
-        <v>18</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="9">
-        <v>19</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="90">
+      <c r="E22" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="90">
       <c r="A23" s="9">
         <v>21</v>
       </c>
       <c r="B23" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>75</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="90">
+    <row r="24" spans="1:8" ht="90">
       <c r="A24" s="9">
         <v>22</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:8">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="30">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="30">
       <c r="A27" s="9">
         <v>25</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:8">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="9">
         <v>27</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="30">
+      <c r="H29" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="45">
       <c r="A30" s="9">
         <v>28</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
+      <c r="E30" s="10" t="s">
+        <v>101</v>
+      </c>
       <c r="F30" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="J30" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="60">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="60">
       <c r="A32" s="9">
         <v>30</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="9">
+        <v>31</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D33" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Populator fill in ProgramStr
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="111">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -407,6 +407,17 @@
   </si>
   <si>
     <t>用strikethrough代替gray</t>
+  </si>
+  <si>
+    <t>TR的ProStr和SubStr没有赋值</t>
+  </si>
+  <si>
+    <t>之前没用到，所以没有做也没发现</t>
+  </si>
+  <si>
+    <t>TR的创建，是在Create或SaveAs Program的时候完成的。具体来说是在ProgramEditView里面。
+Create：Add的时候，通过template创建TR，此时应将SubStr赋值。OK的时候，对ProStr赋值。
+SaveAs: Clone的时候对SubStr赋值。OK的时候，对ProStr赋值。</t>
   </si>
 </sst>
 </file>
@@ -901,7 +912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -1077,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E37" sqref="E36:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1620,6 +1631,20 @@
         <v>13</v>
       </c>
     </row>
+    <row r="35" spans="1:6" ht="90">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Replace status with Use Count
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -1000,7 +1000,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1297,10 +1297,10 @@
       <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="13" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sub Program Added Loop
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="136">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -495,10 +495,11 @@
 Populator那边作相应的修改。</t>
   </si>
   <si>
-    <t>model加上loop属性。View Model加上wraper。View加上UI。Populator作相应修改。</t>
-  </si>
-  <si>
     <t>Sub Program加上Loop选项</t>
+  </si>
+  <si>
+    <t>model加上loop属性。View Model加上wraper。View加上UI。Populator作相应修改。
+ProgramEditView这边还得修改</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1047,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+      <selection activeCell="D14" sqref="D14:S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1490,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1908,6 +1909,9 @@
       <c r="B25" s="17" t="s">
         <v>79</v>
       </c>
+      <c r="F25" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26" spans="1:10" ht="30">
       <c r="A26" s="3">
@@ -2086,6 +2090,9 @@
       <c r="B36" s="17" t="s">
         <v>120</v>
       </c>
+      <c r="F36" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="7">
@@ -2094,6 +2101,9 @@
       <c r="B37" s="17" t="s">
         <v>122</v>
       </c>
+      <c r="F37" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="7">
@@ -2102,6 +2112,9 @@
       <c r="B38" s="17" t="s">
         <v>127</v>
       </c>
+      <c r="F38" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="7">
@@ -2109,6 +2122,9 @@
       </c>
       <c r="B39" s="17" t="s">
         <v>130</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="90">
@@ -2134,16 +2150,24 @@
       <c r="B41" s="17" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="30">
-      <c r="A42" s="7">
+      <c r="F41" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="45">
+      <c r="A42" s="3">
         <v>40</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="E42" s="17" t="s">
-        <v>134</v>
+      <c r="F42" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solution 3 of item44
</commit_message>
<xml_diff>
--- a/Doc/Issue List.xlsx
+++ b/Doc/Issue List.xlsx
@@ -540,7 +540,8 @@
   <si>
     <t>方案1：VM在commit的时候强行更新所有Pro的ET。简单粗暴，但不是特别合理。如果Pro特别多呢？会有性能问题。
 方案2：给program model加上et属性，vm从m获得et属性。Commit的时候更新m的et，从而更新vm和v。P.commit需要pros，从vm传下去给m。（参考41）
-采用方案2</t>
+方案3，即不在db解决问题，也不在model解决问题，而仅仅在vm层解决问题。把et理解为纯ui，跟业务逻辑无关。
+方案2跟方案3的区别在于，方案2使得et存在于model层，方案3的model层里没有et。方案选择的关键在于如何看待et。目前的需求来说，et只是UI显示用一下，没有其他用途，所以选择方案3</t>
   </si>
 </sst>
 </file>
@@ -1535,7 +1536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
@@ -2261,21 +2262,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="105">
-      <c r="A46" s="7">
+    <row r="46" spans="1:8" ht="180">
+      <c r="A46" s="3">
         <v>44</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="C46" s="13"/>
+      <c r="D46" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="E46" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="F46" s="8" t="s">
-        <v>13</v>
+      <c r="F46" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>